<commit_message>
Changing appinfo.py to config.py. Initial implementation (well and lease) of sqlite_objects + relevant tests.
</commit_message>
<xml_diff>
--- a/excel-app/files/test_database.xlsx
+++ b/excel-app/files/test_database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="978" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Royalty Master" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>LeaseType</t>
   </si>
@@ -180,6 +180,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -279,12 +280,12 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="A1:J9 C21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,15 +578,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:J9"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,19 +602,25 @@
       <c r="D1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>30</v>
       </c>
     </row>
@@ -631,18 +638,24 @@
         <v>33</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <v>41974</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -660,18 +673,24 @@
         <v>33</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
         <v>41974</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -689,12 +708,18 @@
         <v>33</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -712,12 +737,18 @@
         <v>33</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -735,9 +766,15 @@
         <v>45</v>
       </c>
       <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -755,15 +792,21 @@
         <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="n">
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="n">
         <v>41974</v>
       </c>
     </row>
@@ -781,15 +824,21 @@
         <v>33</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="n">
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="n">
         <v>41974</v>
       </c>
     </row>
@@ -807,22 +856,28 @@
         <v>33</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="n">
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="n">
         <v>41974</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>